<commit_message>
edits to projects (can handle suffix)
</commit_message>
<xml_diff>
--- a/DatasetTemplate.xlsx
+++ b/DatasetTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kristina\ephys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kristina\git local\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B5CFAF-5538-4B17-AA7F-3B9B0B47EF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EF6B2D-85EC-4369-BDF6-2C944417C0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2240" windowWidth="31800" windowHeight="19360" activeTab="1" xr2:uid="{D3CEA0B0-3692-4CBE-808C-13B3C67ED86B}"/>
+    <workbookView xWindow="620" yWindow="830" windowWidth="31800" windowHeight="19360" activeTab="1" xr2:uid="{D3CEA0B0-3692-4CBE-808C-13B3C67ED86B}"/>
   </bookViews>
   <sheets>
     <sheet name="Search string" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     3 numbers</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{2703FE4F-3088-48FC-8379-DB69258A3A42}">
+    <comment ref="F1" authorId="2" shapeId="0" xr:uid="{2703FE4F-3088-48FC-8379-DB69258A3A42}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Animal</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Initials</t>
+  </si>
+  <si>
+    <t>Suffix</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
   <threadedComment ref="C1" dT="2024-02-23T18:42:30.39" personId="{B17A7428-886E-46B4-B717-AD89107629A6}" id="{12EF3A6C-9AA6-48E2-A198-03ADD7AB9D11}">
     <text>3 numbers</text>
   </threadedComment>
-  <threadedComment ref="E1" dT="2024-02-22T15:45:21.33" personId="{B17A7428-886E-46B4-B717-AD89107629A6}" id="{2703FE4F-3088-48FC-8379-DB69258A3A42}">
+  <threadedComment ref="F1" dT="2024-02-22T15:45:21.33" personId="{B17A7428-886E-46B4-B717-AD89107629A6}" id="{2703FE4F-3088-48FC-8379-DB69258A3A42}">
     <text>SU or MU</text>
   </threadedComment>
 </ThreadedComments>
@@ -587,10 +593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01425243-AC00-415C-A011-4DAA15D1A7B2}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,7 +608,7 @@
     <col min="7" max="7" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,20 +621,31 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>